<commit_message>
DP 39 40 41
</commit_message>
<xml_diff>
--- a/DSA-280.xlsx
+++ b/DSA-280.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DSA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B2CC13-84EC-406C-9C1C-3DD20C2CA94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="328">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -510,17 +519,19 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-        <u/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -1007,110 +1018,133 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/count-of-range-sum/</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12.0"/>
-      <color rgb="FF1155CC"/>
-    </font>
-    <font>
-      <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="&quot;Open Sans&quot;"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="&quot;Open Sans&quot;"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="&quot;Open Sans&quot;"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1118,7 +1152,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1128,90 +1162,73 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1401,29 +1418,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="29.25"/>
-    <col customWidth="1" min="2" max="2" width="65.88"/>
-    <col customWidth="1" min="3" max="3" width="27.38"/>
-    <col customWidth="1" min="4" max="4" width="16.0"/>
-    <col customWidth="1" min="5" max="5" width="14.88"/>
-    <col customWidth="1" min="6" max="6" width="15.25"/>
-    <col customWidth="1" min="8" max="8" width="20.13"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="65.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1434,10 +1456,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="13.2">
       <c r="I2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="13.2">
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1457,7 +1479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="13.2">
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1466,62 +1488,80 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="13.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="C5" t="s">
+        <v>327</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="13.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="C6" t="s">
+        <v>327</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="13.2">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="C7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13.2">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="C8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="13.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="C9" t="s">
+        <v>327</v>
+      </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="13.2">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>327</v>
+      </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1529,13 +1569,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="13.2">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="C11" t="s">
+        <v>327</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1543,45 +1586,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="13.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C12" t="s">
+        <v>327</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" ht="13.2">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="C13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="13.2">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="C14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="13.2">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="C15" t="s">
+        <v>327</v>
+      </c>
       <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" ht="13.2">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -1595,13 +1650,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="13.2">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="C17" t="s">
+        <v>327</v>
+      </c>
       <c r="E17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1609,15 +1667,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="13.2">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="C18" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="13.2">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -1625,45 +1686,57 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="13.2">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="C20" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13.2">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="C21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="13.2">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="C22" t="s">
+        <v>327</v>
+      </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="13.2">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="C23" t="s">
+        <v>327</v>
+      </c>
       <c r="G23" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" ht="13.2">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" ht="13.2">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -1685,7 +1758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" ht="13.2">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
@@ -1696,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
@@ -1704,7 +1777,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="13.2">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1712,7 +1785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" ht="13.2">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
@@ -1720,7 +1793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" ht="13.2">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -1728,7 +1801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" ht="13.2">
       <c r="A31" s="4" t="s">
         <v>37</v>
       </c>
@@ -1739,7 +1812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="13.2">
       <c r="A32" s="4" t="s">
         <v>37</v>
       </c>
@@ -1748,16 +1821,16 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" ht="13.2">
       <c r="D33" s="4"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" ht="13.2">
       <c r="B34" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" ht="13.2">
       <c r="A35" s="4" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1838,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" ht="13.2">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
@@ -1776,7 +1849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" ht="13.2">
       <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
@@ -1784,7 +1857,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" ht="13.2">
       <c r="A38" s="4" t="s">
         <v>11</v>
       </c>
@@ -1795,7 +1868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" ht="13.2">
       <c r="A39" s="4" t="s">
         <v>11</v>
       </c>
@@ -1803,7 +1876,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" ht="13.2">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -1814,7 +1887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" ht="13.2">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
@@ -1825,7 +1898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" ht="13.2">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
@@ -1839,7 +1912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" ht="13.2">
       <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
@@ -1850,7 +1923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" ht="13.2">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
@@ -1861,7 +1934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" ht="13.2">
       <c r="A45" s="4" t="s">
         <v>47</v>
       </c>
@@ -1869,7 +1942,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" ht="13.2">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -1877,7 +1950,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" ht="13.2">
       <c r="A47" s="4" t="s">
         <v>47</v>
       </c>
@@ -1885,7 +1958,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" ht="13.2">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -1893,7 +1966,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" ht="13.2">
       <c r="A49" s="4" t="s">
         <v>37</v>
       </c>
@@ -1901,7 +1974,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" ht="13.2">
       <c r="A50" s="4" t="s">
         <v>37</v>
       </c>
@@ -1912,7 +1985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" ht="13.2">
       <c r="A51" s="4" t="s">
         <v>37</v>
       </c>
@@ -1923,7 +1996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" ht="13.2">
       <c r="A52" s="4" t="s">
         <v>37</v>
       </c>
@@ -1934,7 +2007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" ht="13.2">
       <c r="A53" s="4" t="s">
         <v>37</v>
       </c>
@@ -1942,7 +2015,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" ht="13.2">
       <c r="A54" s="4" t="s">
         <v>37</v>
       </c>
@@ -1950,12 +2023,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" ht="13.2">
       <c r="H55" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" ht="13.2">
       <c r="B56" s="3" t="s">
         <v>63</v>
       </c>
@@ -1963,7 +2036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" ht="13.2">
       <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +2047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" ht="13.2">
       <c r="A58" s="4" t="s">
         <v>21</v>
       </c>
@@ -1982,7 +2055,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" ht="13.2">
       <c r="A59" s="4" t="s">
         <v>21</v>
       </c>
@@ -1993,7 +2066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" ht="13.2">
       <c r="A60" s="4" t="s">
         <v>21</v>
       </c>
@@ -2001,7 +2074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" ht="13.2">
       <c r="A61" s="4" t="s">
         <v>21</v>
       </c>
@@ -2012,16 +2085,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" ht="13.2">
       <c r="G62" s="4"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" ht="13.2">
       <c r="B63" s="4" t="s">
         <v>68</v>
       </c>
       <c r="G63" s="4"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" ht="13.2">
       <c r="A64" s="4" t="s">
         <v>11</v>
       </c>
@@ -2029,7 +2102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" ht="13.2">
       <c r="A65" s="4" t="s">
         <v>11</v>
       </c>
@@ -2040,7 +2113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" ht="13.2">
       <c r="A66" s="4" t="s">
         <v>11</v>
       </c>
@@ -2051,7 +2124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:8" ht="13.2">
       <c r="A67" s="4" t="s">
         <v>11</v>
       </c>
@@ -2059,7 +2132,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:8" ht="13.2">
       <c r="A68" s="4" t="s">
         <v>11</v>
       </c>
@@ -2067,7 +2140,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" ht="13.2">
       <c r="A69" s="4" t="s">
         <v>11</v>
       </c>
@@ -2078,7 +2151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:8" ht="13.2">
       <c r="A70" s="4" t="s">
         <v>11</v>
       </c>
@@ -2089,7 +2162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:8" ht="13.2">
       <c r="A71" s="4" t="s">
         <v>11</v>
       </c>
@@ -2100,7 +2173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:8" ht="13.2">
       <c r="A72" s="4" t="s">
         <v>11</v>
       </c>
@@ -2111,7 +2184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:8" ht="13.2">
       <c r="A73" s="4" t="s">
         <v>21</v>
       </c>
@@ -2122,7 +2195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:8" ht="13.2">
       <c r="A74" s="4" t="s">
         <v>21</v>
       </c>
@@ -2133,7 +2206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:8" ht="13.2">
       <c r="A75" s="4" t="s">
         <v>21</v>
       </c>
@@ -2147,12 +2220,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:8" ht="13.2">
       <c r="B77" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="4" t="s">
         <v>11</v>
       </c>
@@ -2163,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:8" ht="13.2">
       <c r="A79" s="4" t="s">
         <v>11</v>
       </c>
@@ -2171,7 +2244,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="4" t="s">
         <v>11</v>
       </c>
@@ -2179,7 +2252,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:7" ht="13.2">
       <c r="A81" s="4" t="s">
         <v>11</v>
       </c>
@@ -2190,7 +2263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:7" ht="15">
       <c r="A82" s="4" t="s">
         <v>21</v>
       </c>
@@ -2201,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:7" ht="15">
       <c r="A83" s="4" t="s">
         <v>21</v>
       </c>
@@ -2212,7 +2285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:7" ht="13.2">
       <c r="A84" s="4" t="s">
         <v>21</v>
       </c>
@@ -2226,7 +2299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:7" ht="15">
       <c r="A85" s="4" t="s">
         <v>21</v>
       </c>
@@ -2240,7 +2313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:7" ht="15">
       <c r="A86" s="4" t="s">
         <v>21</v>
       </c>
@@ -2251,7 +2324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:7" ht="13.2">
       <c r="A87" s="4" t="s">
         <v>37</v>
       </c>
@@ -2262,7 +2335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:7" ht="13.2">
       <c r="A88" s="4" t="s">
         <v>37</v>
       </c>
@@ -2273,7 +2346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:7" ht="13.2">
       <c r="A89" s="4" t="s">
         <v>37</v>
       </c>
@@ -2281,7 +2354,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:7" ht="15">
       <c r="A90" s="4" t="s">
         <v>37</v>
       </c>
@@ -2289,7 +2362,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:7" ht="15">
       <c r="A91" s="4" t="s">
         <v>37</v>
       </c>
@@ -2300,7 +2373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:7" ht="15">
       <c r="A92" s="4" t="s">
         <v>37</v>
       </c>
@@ -2308,15 +2381,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:7" ht="15">
       <c r="B93" s="12"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:7" ht="13.2">
       <c r="B95" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:7" ht="13.2">
       <c r="A96" s="4" t="s">
         <v>11</v>
       </c>
@@ -2330,7 +2403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:8" ht="13.2">
       <c r="A97" s="4" t="s">
         <v>11</v>
       </c>
@@ -2341,7 +2414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:8" ht="13.2">
       <c r="A98" s="4" t="s">
         <v>11</v>
       </c>
@@ -2355,7 +2428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:8" ht="13.2">
       <c r="A99" s="4" t="s">
         <v>11</v>
       </c>
@@ -2366,7 +2439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:8" ht="13.2">
       <c r="A100" s="4" t="s">
         <v>11</v>
       </c>
@@ -2377,7 +2450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:8" ht="13.2">
       <c r="A101" s="4" t="s">
         <v>11</v>
       </c>
@@ -2388,7 +2461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:8" ht="13.2">
       <c r="A102" s="4" t="s">
         <v>11</v>
       </c>
@@ -2405,7 +2478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:8" ht="13.2">
       <c r="A103" s="4" t="s">
         <v>11</v>
       </c>
@@ -2416,7 +2489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:8" ht="13.2">
       <c r="A104" s="4" t="s">
         <v>11</v>
       </c>
@@ -2424,7 +2497,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:8" ht="13.2">
       <c r="A105" s="4" t="s">
         <v>11</v>
       </c>
@@ -2435,7 +2508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:8" ht="13.2">
       <c r="A106" s="4" t="s">
         <v>11</v>
       </c>
@@ -2446,7 +2519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:8" ht="13.2">
       <c r="A107" s="4" t="s">
         <v>11</v>
       </c>
@@ -2457,7 +2530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:8" ht="13.2">
       <c r="A108" s="4" t="s">
         <v>21</v>
       </c>
@@ -2468,7 +2541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:8" ht="13.2">
       <c r="A109" s="4" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:8" ht="13.2">
       <c r="A110" s="4" t="s">
         <v>21</v>
       </c>
@@ -2490,7 +2563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:8" ht="13.2">
       <c r="A111" s="4" t="s">
         <v>21</v>
       </c>
@@ -2498,7 +2571,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:8" ht="13.2">
       <c r="A112" s="4" t="s">
         <v>21</v>
       </c>
@@ -2506,7 +2579,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:8" ht="13.2">
       <c r="A113" s="4" t="s">
         <v>21</v>
       </c>
@@ -2517,7 +2590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:8" ht="13.2">
       <c r="A114" s="4" t="s">
         <v>21</v>
       </c>
@@ -2528,7 +2601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:8" ht="13.2">
       <c r="A115" s="4" t="s">
         <v>21</v>
       </c>
@@ -2539,7 +2612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:8" ht="13.2">
       <c r="A116" s="4" t="s">
         <v>21</v>
       </c>
@@ -2550,7 +2623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:8" ht="13.2">
       <c r="A117" s="4" t="s">
         <v>21</v>
       </c>
@@ -2561,7 +2634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:8" ht="13.2">
       <c r="A118" s="4" t="s">
         <v>21</v>
       </c>
@@ -2572,7 +2645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:8" ht="13.2">
       <c r="A119" s="4" t="s">
         <v>21</v>
       </c>
@@ -2580,7 +2653,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:8" ht="13.2">
       <c r="A120" s="4" t="s">
         <v>21</v>
       </c>
@@ -2591,7 +2664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:8" ht="13.2">
       <c r="A121" s="4" t="s">
         <v>37</v>
       </c>
@@ -2599,7 +2672,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:8" ht="13.2">
       <c r="A122" s="4" t="s">
         <v>37</v>
       </c>
@@ -2610,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:8" ht="13.2">
       <c r="A123" s="4" t="s">
         <v>37</v>
       </c>
@@ -2621,7 +2694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:8" ht="13.2">
       <c r="A124" s="4" t="s">
         <v>37</v>
       </c>
@@ -2632,7 +2705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:8" ht="13.2">
       <c r="A125" s="4" t="s">
         <v>37</v>
       </c>
@@ -2646,12 +2719,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:8" ht="13.2">
       <c r="D126" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:8" ht="13.2">
       <c r="B127" s="13" t="s">
         <v>127</v>
       </c>
@@ -2659,10 +2732,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:8" ht="13.2">
       <c r="B128" s="9"/>
     </row>
-    <row r="129">
+    <row r="129" spans="1:8" ht="13.2">
       <c r="A129" s="4" t="s">
         <v>11</v>
       </c>
@@ -2673,7 +2746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:8" ht="13.2">
       <c r="A130" s="4" t="s">
         <v>11</v>
       </c>
@@ -2687,7 +2760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:8" ht="13.2">
       <c r="A131" s="4" t="s">
         <v>11</v>
       </c>
@@ -2698,7 +2771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:8" ht="13.2">
       <c r="A132" s="4" t="s">
         <v>11</v>
       </c>
@@ -2712,7 +2785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:8" ht="13.2">
       <c r="A133" s="4" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +2799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:8" ht="13.2">
       <c r="A134" s="4" t="s">
         <v>11</v>
       </c>
@@ -2740,7 +2813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:8" ht="13.2">
       <c r="A135" s="4" t="s">
         <v>11</v>
       </c>
@@ -2751,7 +2824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:8" ht="13.2">
       <c r="A136" s="4" t="s">
         <v>21</v>
       </c>
@@ -2759,7 +2832,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:8" ht="13.2">
       <c r="A137" s="4" t="s">
         <v>21</v>
       </c>
@@ -2767,7 +2840,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:8" ht="13.2">
       <c r="A138" s="4" t="s">
         <v>21</v>
       </c>
@@ -2775,7 +2848,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:8" ht="13.2">
       <c r="A139" s="4" t="s">
         <v>21</v>
       </c>
@@ -2786,7 +2859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:8" ht="13.2">
       <c r="A140" s="4" t="s">
         <v>21</v>
       </c>
@@ -2800,7 +2873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:8" ht="13.2">
       <c r="A141" s="4" t="s">
         <v>21</v>
       </c>
@@ -2814,7 +2887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:8" ht="13.2">
       <c r="A142" s="4" t="s">
         <v>21</v>
       </c>
@@ -2825,7 +2898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:8" ht="13.2">
       <c r="A143" s="4" t="s">
         <v>21</v>
       </c>
@@ -2833,7 +2906,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:8" ht="13.2">
       <c r="A144" s="4" t="s">
         <v>21</v>
       </c>
@@ -2841,7 +2914,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:8" ht="13.2">
       <c r="A145" s="4" t="s">
         <v>21</v>
       </c>
@@ -2852,7 +2925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:8" ht="13.2">
       <c r="A146" s="4" t="s">
         <v>37</v>
       </c>
@@ -2863,7 +2936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:8" ht="13.2">
       <c r="A147" s="4" t="s">
         <v>37</v>
       </c>
@@ -2874,7 +2947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:8" ht="13.2">
       <c r="A148" s="4" t="s">
         <v>37</v>
       </c>
@@ -2882,12 +2955,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:8" ht="13.2">
       <c r="B151" s="19" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:8" ht="13.2">
       <c r="A152" s="4" t="s">
         <v>11</v>
       </c>
@@ -2898,7 +2971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:8" ht="13.2">
       <c r="A153" s="4" t="s">
         <v>11</v>
       </c>
@@ -2909,7 +2982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:8" ht="13.2">
       <c r="A154" s="4" t="s">
         <v>11</v>
       </c>
@@ -2920,7 +2993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:8" ht="13.2">
       <c r="A155" s="4" t="s">
         <v>11</v>
       </c>
@@ -2928,7 +3001,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:8" ht="13.2">
       <c r="A156" s="4" t="s">
         <v>11</v>
       </c>
@@ -2936,7 +3009,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:8" ht="13.2">
       <c r="A157" s="4" t="s">
         <v>11</v>
       </c>
@@ -2947,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:8" ht="13.2">
       <c r="A158" s="4" t="s">
         <v>11</v>
       </c>
@@ -2958,7 +3031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:8" ht="13.2">
       <c r="A159" s="4" t="s">
         <v>11</v>
       </c>
@@ -2969,7 +3042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:8" ht="13.2">
       <c r="A160" s="4" t="s">
         <v>11</v>
       </c>
@@ -2980,7 +3053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:6" ht="13.2">
       <c r="A161" s="4" t="s">
         <v>11</v>
       </c>
@@ -2991,7 +3064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:6" ht="13.2">
       <c r="A162" s="4" t="s">
         <v>11</v>
       </c>
@@ -3002,7 +3075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:6" ht="13.2">
       <c r="A163" s="4" t="s">
         <v>11</v>
       </c>
@@ -3010,7 +3083,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:6" ht="13.2">
       <c r="A164" s="4" t="s">
         <v>11</v>
       </c>
@@ -3018,7 +3091,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:6" ht="13.2">
       <c r="A165" s="4" t="s">
         <v>11</v>
       </c>
@@ -3026,7 +3099,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:6" ht="13.2">
       <c r="A166" s="4" t="s">
         <v>11</v>
       </c>
@@ -3034,7 +3107,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:6" ht="13.2">
       <c r="A167" s="4" t="s">
         <v>11</v>
       </c>
@@ -3042,7 +3115,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:6" ht="13.2">
       <c r="A168" s="4" t="s">
         <v>11</v>
       </c>
@@ -3050,7 +3123,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:6" ht="13.2">
       <c r="A169" s="4" t="s">
         <v>11</v>
       </c>
@@ -3058,7 +3131,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:6" ht="13.2">
       <c r="A170" s="4" t="s">
         <v>21</v>
       </c>
@@ -3066,7 +3139,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:6" ht="13.2">
       <c r="A171" s="4" t="s">
         <v>21</v>
       </c>
@@ -3077,7 +3150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:6" ht="13.2">
       <c r="A172" s="4" t="s">
         <v>21</v>
       </c>
@@ -3088,7 +3161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:6" ht="13.2">
       <c r="A173" s="4" t="s">
         <v>21</v>
       </c>
@@ -3099,7 +3172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:6" ht="13.2">
       <c r="A174" s="4" t="s">
         <v>21</v>
       </c>
@@ -3107,7 +3180,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:6" ht="13.2">
       <c r="A175" s="4" t="s">
         <v>21</v>
       </c>
@@ -3115,7 +3188,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:6" ht="13.2">
       <c r="A176" s="4" t="s">
         <v>21</v>
       </c>
@@ -3123,7 +3196,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:6" ht="13.2">
       <c r="A177" s="4" t="s">
         <v>21</v>
       </c>
@@ -3134,7 +3207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:6" ht="13.2">
       <c r="A178" s="4" t="s">
         <v>21</v>
       </c>
@@ -3148,7 +3221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:6" ht="13.2">
       <c r="A179" s="4" t="s">
         <v>21</v>
       </c>
@@ -3162,7 +3235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:6" ht="13.2">
       <c r="A180" s="4" t="s">
         <v>21</v>
       </c>
@@ -3173,7 +3246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:6" ht="13.2">
       <c r="A181" s="4" t="s">
         <v>21</v>
       </c>
@@ -3181,7 +3254,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:6" ht="13.2">
       <c r="A182" s="4" t="s">
         <v>21</v>
       </c>
@@ -3189,7 +3262,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:6" ht="13.2">
       <c r="A183" s="4" t="s">
         <v>21</v>
       </c>
@@ -3197,7 +3270,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:6" ht="13.2">
       <c r="A184" s="4" t="s">
         <v>21</v>
       </c>
@@ -3208,7 +3281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:6" ht="13.2">
       <c r="A185" s="4" t="s">
         <v>21</v>
       </c>
@@ -3219,7 +3292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:6" ht="13.2">
       <c r="A186" s="4" t="s">
         <v>21</v>
       </c>
@@ -3230,7 +3303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:6" ht="13.2">
       <c r="A187" s="4" t="s">
         <v>21</v>
       </c>
@@ -3241,7 +3314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:6" ht="13.2">
       <c r="A188" s="4" t="s">
         <v>21</v>
       </c>
@@ -3249,7 +3322,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:6" ht="13.2">
       <c r="A189" s="4" t="s">
         <v>21</v>
       </c>
@@ -3260,7 +3333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:6" ht="13.2">
       <c r="A190" s="4" t="s">
         <v>37</v>
       </c>
@@ -3268,7 +3341,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:6" ht="13.2">
       <c r="A191" s="4" t="s">
         <v>37</v>
       </c>
@@ -3276,7 +3349,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:6" ht="13.2">
       <c r="A192" s="4" t="s">
         <v>37</v>
       </c>
@@ -3287,7 +3360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:8" ht="13.2">
       <c r="A193" s="4" t="s">
         <v>37</v>
       </c>
@@ -3301,7 +3374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:8" ht="13.2">
       <c r="A194" s="4" t="s">
         <v>37</v>
       </c>
@@ -3318,7 +3391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:8" ht="13.2">
       <c r="A195" s="4" t="s">
         <v>37</v>
       </c>
@@ -3326,7 +3399,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:8" ht="13.2">
       <c r="A196" s="4" t="s">
         <v>37</v>
       </c>
@@ -3334,7 +3407,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:8" ht="13.2">
       <c r="A197" s="4" t="s">
         <v>37</v>
       </c>
@@ -3345,7 +3418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:8" ht="13.2">
       <c r="A198" s="4" t="s">
         <v>37</v>
       </c>
@@ -3356,7 +3429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:8" ht="13.2">
       <c r="A199" s="4" t="s">
         <v>37</v>
       </c>
@@ -3364,12 +3437,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:8" ht="13.2">
       <c r="B201" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:8" ht="13.2">
       <c r="A202" s="4" t="s">
         <v>11</v>
       </c>
@@ -3377,7 +3450,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:8" ht="13.2">
       <c r="A203" s="4" t="s">
         <v>11</v>
       </c>
@@ -3388,7 +3461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:8" ht="13.2">
       <c r="A204" s="4" t="s">
         <v>11</v>
       </c>
@@ -3399,7 +3472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:8" ht="13.2">
       <c r="A205" s="4" t="s">
         <v>11</v>
       </c>
@@ -3410,7 +3483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:8" ht="13.2">
       <c r="A206" s="4" t="s">
         <v>11</v>
       </c>
@@ -3421,7 +3494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:8" ht="13.2">
       <c r="A207" s="4" t="s">
         <v>11</v>
       </c>
@@ -3432,7 +3505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:8" ht="13.2">
       <c r="A208" s="4" t="s">
         <v>11</v>
       </c>
@@ -3443,7 +3516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:8" ht="13.2">
       <c r="A209" s="4" t="s">
         <v>21</v>
       </c>
@@ -3451,7 +3524,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:8" ht="13.2">
       <c r="A210" s="4" t="s">
         <v>21</v>
       </c>
@@ -3462,7 +3535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:8" ht="13.2">
       <c r="A211" s="4" t="s">
         <v>21</v>
       </c>
@@ -3476,7 +3549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:8" ht="13.2">
       <c r="A212" s="4" t="s">
         <v>21</v>
       </c>
@@ -3487,7 +3560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:8" ht="13.2">
       <c r="A213" s="4" t="s">
         <v>21</v>
       </c>
@@ -3495,7 +3568,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:8" ht="13.2">
       <c r="A214" s="4" t="s">
         <v>21</v>
       </c>
@@ -3506,7 +3579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:8" ht="13.2">
       <c r="A215" s="4" t="s">
         <v>21</v>
       </c>
@@ -3517,7 +3590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:8" ht="13.2">
       <c r="A216" s="4" t="s">
         <v>21</v>
       </c>
@@ -3525,7 +3598,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:8" ht="13.2">
       <c r="A217" s="4" t="s">
         <v>21</v>
       </c>
@@ -3533,7 +3606,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:8" ht="13.2">
       <c r="A218" s="4" t="s">
         <v>21</v>
       </c>
@@ -3541,7 +3614,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:8" ht="13.2">
       <c r="A219" s="4" t="s">
         <v>21</v>
       </c>
@@ -3552,7 +3625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:8" ht="13.2">
       <c r="A220" s="4" t="s">
         <v>21</v>
       </c>
@@ -3563,7 +3636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:8" ht="13.2">
       <c r="A221" s="4" t="s">
         <v>21</v>
       </c>
@@ -3577,7 +3650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:8" ht="13.2">
       <c r="A222" s="4" t="s">
         <v>21</v>
       </c>
@@ -3588,7 +3661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:8" ht="13.2">
       <c r="A223" s="4" t="s">
         <v>21</v>
       </c>
@@ -3599,7 +3672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:8" ht="13.2">
       <c r="A224" s="4" t="s">
         <v>21</v>
       </c>
@@ -3610,7 +3683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:8" ht="13.2">
       <c r="A225" s="4" t="s">
         <v>21</v>
       </c>
@@ -3621,7 +3694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:8" ht="13.2">
       <c r="A226" s="4" t="s">
         <v>21</v>
       </c>
@@ -3632,7 +3705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:8" ht="13.2">
       <c r="A227" s="4" t="s">
         <v>21</v>
       </c>
@@ -3643,7 +3716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:8" ht="13.2">
       <c r="A228" s="4" t="s">
         <v>21</v>
       </c>
@@ -3654,7 +3727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:8" ht="13.2">
       <c r="A229" s="4" t="s">
         <v>37</v>
       </c>
@@ -3665,7 +3738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:8" ht="13.2">
       <c r="A230" s="4" t="s">
         <v>37</v>
       </c>
@@ -3676,7 +3749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:8" ht="13.2">
       <c r="A231" s="4" t="s">
         <v>37</v>
       </c>
@@ -3684,7 +3757,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:8" ht="13.2">
       <c r="A232" s="4" t="s">
         <v>37</v>
       </c>
@@ -3692,7 +3765,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:8" ht="13.2">
       <c r="A233" s="4" t="s">
         <v>37</v>
       </c>
@@ -3703,7 +3776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:8" ht="13.2">
       <c r="A234" s="4" t="s">
         <v>37</v>
       </c>
@@ -3714,7 +3787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:8" ht="13.2">
       <c r="A235" s="4" t="s">
         <v>37</v>
       </c>
@@ -3725,7 +3798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:8" ht="13.2">
       <c r="A236" s="4" t="s">
         <v>37</v>
       </c>
@@ -3736,7 +3809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:8" ht="13.2">
       <c r="A237" s="4" t="s">
         <v>37</v>
       </c>
@@ -3747,7 +3820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:8" ht="13.2">
       <c r="A238" s="4" t="s">
         <v>37</v>
       </c>
@@ -3755,17 +3828,17 @@
         <v>234</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:8" ht="13.2">
       <c r="D239" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:8" ht="13.2">
       <c r="B240" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:8" ht="13.2">
       <c r="A241" s="4" t="s">
         <v>21</v>
       </c>
@@ -3776,7 +3849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:8" ht="13.2">
       <c r="A242" s="4" t="s">
         <v>21</v>
       </c>
@@ -3790,7 +3863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:8" ht="13.2">
       <c r="A243" s="4" t="s">
         <v>21</v>
       </c>
@@ -3801,7 +3874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:8" ht="13.2">
       <c r="A244" s="4" t="s">
         <v>21</v>
       </c>
@@ -3809,7 +3882,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:8" ht="13.2">
       <c r="A245" s="4" t="s">
         <v>37</v>
       </c>
@@ -3820,7 +3893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:8" ht="13.2">
       <c r="A246" s="4" t="s">
         <v>37</v>
       </c>
@@ -3829,18 +3902,18 @@
       </c>
       <c r="D246" s="4"/>
     </row>
-    <row r="247">
+    <row r="247" spans="1:8" ht="13.2">
       <c r="D247" s="4"/>
       <c r="H247" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:8" ht="13.2">
       <c r="B248" s="20" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" spans="1:8" ht="13.2">
       <c r="A250" s="4" t="s">
         <v>243</v>
       </c>
@@ -3848,7 +3921,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:8" ht="13.2">
       <c r="A251" s="4" t="s">
         <v>243</v>
       </c>
@@ -3859,7 +3932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:8" ht="13.2">
       <c r="A252" s="4" t="s">
         <v>243</v>
       </c>
@@ -3870,7 +3943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:8" ht="13.2">
       <c r="A253" s="4" t="s">
         <v>243</v>
       </c>
@@ -3881,7 +3954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:8" ht="13.2">
       <c r="A254" s="4" t="s">
         <v>243</v>
       </c>
@@ -3889,7 +3962,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:8" ht="13.2">
       <c r="A255" s="4" t="s">
         <v>243</v>
       </c>
@@ -3903,7 +3976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:8" ht="13.2">
       <c r="A256" s="4" t="s">
         <v>243</v>
       </c>
@@ -3911,7 +3984,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:8" ht="13.2">
       <c r="A257" s="4" t="s">
         <v>243</v>
       </c>
@@ -3925,7 +3998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:8" ht="13.2">
       <c r="A258" s="4" t="s">
         <v>243</v>
       </c>
@@ -3939,7 +4012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:8" ht="13.2">
       <c r="A259" s="4" t="s">
         <v>243</v>
       </c>
@@ -3947,7 +4020,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="1:8" ht="13.2">
       <c r="A260" s="4" t="s">
         <v>37</v>
       </c>
@@ -3955,7 +4028,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:8" ht="13.2">
       <c r="A261" s="4" t="s">
         <v>37</v>
       </c>
@@ -3969,7 +4042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:8" ht="13.2">
       <c r="A262" s="4" t="s">
         <v>37</v>
       </c>
@@ -3977,7 +4050,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:8" ht="13.2">
       <c r="A263" s="4" t="s">
         <v>37</v>
       </c>
@@ -3994,12 +4067,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:8" ht="13.2">
       <c r="B265" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:8" ht="13.2">
       <c r="A266" s="4" t="s">
         <v>11</v>
       </c>
@@ -4007,7 +4080,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:8" ht="13.2">
       <c r="A267" s="4" t="s">
         <v>11</v>
       </c>
@@ -4015,7 +4088,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:8" ht="13.2">
       <c r="A268" s="4" t="s">
         <v>11</v>
       </c>
@@ -4023,7 +4096,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:8" ht="13.2">
       <c r="A269" s="4" t="s">
         <v>11</v>
       </c>
@@ -4034,7 +4107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="1:8" ht="13.2">
       <c r="A270" s="4" t="s">
         <v>21</v>
       </c>
@@ -4048,7 +4121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:8" ht="13.2">
       <c r="A271" s="4" t="s">
         <v>21</v>
       </c>
@@ -4062,7 +4135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:8" ht="13.2">
       <c r="A272" s="4" t="s">
         <v>21</v>
       </c>
@@ -4070,7 +4143,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="1:8" ht="13.2">
       <c r="A273" s="4" t="s">
         <v>21</v>
       </c>
@@ -4078,7 +4151,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="1:8" ht="13.2">
       <c r="A274" s="4" t="s">
         <v>21</v>
       </c>
@@ -4086,7 +4159,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:8" ht="13.2">
       <c r="A275" s="4" t="s">
         <v>21</v>
       </c>
@@ -4100,7 +4173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="1:8" ht="13.2">
       <c r="A276" s="4" t="s">
         <v>21</v>
       </c>
@@ -4114,7 +4187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="1:8" ht="13.2">
       <c r="A277" s="4" t="s">
         <v>21</v>
       </c>
@@ -4128,7 +4201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="1:8" ht="13.2">
       <c r="A278" s="4" t="s">
         <v>21</v>
       </c>
@@ -4136,7 +4209,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" spans="1:8" ht="13.2">
       <c r="A279" s="4" t="s">
         <v>21</v>
       </c>
@@ -4144,7 +4217,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="1:8" ht="13.2">
       <c r="A280" s="4" t="s">
         <v>21</v>
       </c>
@@ -4152,7 +4225,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:8" ht="13.2">
       <c r="A281" s="4" t="s">
         <v>21</v>
       </c>
@@ -4166,7 +4239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" spans="1:8" ht="13.2">
       <c r="A282" s="4" t="s">
         <v>21</v>
       </c>
@@ -4174,7 +4247,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:8" ht="13.2">
       <c r="A283" s="4" t="s">
         <v>21</v>
       </c>
@@ -4182,7 +4255,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:8" ht="13.2">
       <c r="A284" s="4" t="s">
         <v>21</v>
       </c>
@@ -4196,7 +4269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:8" ht="13.2">
       <c r="A285" s="4" t="s">
         <v>37</v>
       </c>
@@ -4210,7 +4283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" spans="1:8" ht="13.2">
       <c r="A286" s="4" t="s">
         <v>37</v>
       </c>
@@ -4218,7 +4291,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" spans="1:8" ht="13.2">
       <c r="A287" s="4" t="s">
         <v>37</v>
       </c>
@@ -4229,7 +4302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:8" ht="13.2">
       <c r="A288" s="4" t="s">
         <v>37</v>
       </c>
@@ -4237,7 +4310,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" spans="1:8" ht="13.2">
       <c r="A289" s="4" t="s">
         <v>37</v>
       </c>
@@ -4251,7 +4324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290">
+    <row r="290" spans="1:8" ht="13.2">
       <c r="A290" s="4" t="s">
         <v>37</v>
       </c>
@@ -4262,7 +4335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" spans="1:8" ht="13.2">
       <c r="A291" s="4" t="s">
         <v>37</v>
       </c>
@@ -4276,7 +4349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" spans="1:8" ht="13.2">
       <c r="A292" s="4" t="s">
         <v>37</v>
       </c>
@@ -4284,7 +4357,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" spans="1:8" ht="13.2">
       <c r="A293" s="4" t="s">
         <v>37</v>
       </c>
@@ -4298,7 +4371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" spans="1:8" ht="13.2">
       <c r="A294" s="4" t="s">
         <v>37</v>
       </c>
@@ -4306,7 +4379,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" spans="1:8" ht="13.2">
       <c r="A295" s="4" t="s">
         <v>37</v>
       </c>
@@ -4317,18 +4390,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" spans="1:8" ht="13.2">
       <c r="D296" s="4"/>
       <c r="G296" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" spans="1:8" ht="13.2">
       <c r="B297" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" spans="1:8" ht="13.2">
       <c r="A298" s="4" t="s">
         <v>21</v>
       </c>
@@ -4339,7 +4412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" spans="1:8" ht="13.2">
       <c r="A299" s="4" t="s">
         <v>21</v>
       </c>
@@ -4350,7 +4423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300">
+    <row r="300" spans="1:8" ht="13.2">
       <c r="A300" s="4" t="s">
         <v>21</v>
       </c>
@@ -4361,12 +4434,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303">
+    <row r="303" spans="1:8" ht="13.2">
       <c r="B303" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="304">
+    <row r="304" spans="1:8" ht="13.2">
       <c r="A304" s="4" t="s">
         <v>243</v>
       </c>
@@ -4377,7 +4450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305">
+    <row r="305" spans="1:8" ht="13.2">
       <c r="A305" s="4" t="s">
         <v>243</v>
       </c>
@@ -4391,7 +4464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306">
+    <row r="306" spans="1:8" ht="13.2">
       <c r="A306" s="4" t="s">
         <v>243</v>
       </c>
@@ -4399,7 +4472,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="307">
+    <row r="307" spans="1:8" ht="13.2">
       <c r="A307" s="4" t="s">
         <v>243</v>
       </c>
@@ -4407,7 +4480,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="308">
+    <row r="308" spans="1:8" ht="13.2">
       <c r="A308" s="4" t="s">
         <v>243</v>
       </c>
@@ -4418,7 +4491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309">
+    <row r="309" spans="1:8" ht="13.2">
       <c r="A309" s="4" t="s">
         <v>243</v>
       </c>
@@ -4429,7 +4502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310">
+    <row r="310" spans="1:8" ht="13.2">
       <c r="A310" s="4" t="s">
         <v>243</v>
       </c>
@@ -4440,7 +4513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311">
+    <row r="311" spans="1:8" ht="13.2">
       <c r="A311" s="4" t="s">
         <v>243</v>
       </c>
@@ -4451,7 +4524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312">
+    <row r="312" spans="1:8" ht="13.2">
       <c r="A312" s="4" t="s">
         <v>243</v>
       </c>
@@ -4465,7 +4538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313">
+    <row r="313" spans="1:8" ht="13.2">
       <c r="A313" s="4" t="s">
         <v>243</v>
       </c>
@@ -4482,12 +4555,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316">
+    <row r="316" spans="1:8" ht="13.2">
       <c r="B316" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="317">
+    <row r="317" spans="1:8" ht="13.2">
       <c r="A317" s="4" t="s">
         <v>21</v>
       </c>
@@ -4495,7 +4568,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="318">
+    <row r="318" spans="1:8" ht="13.2">
       <c r="A318" s="4" t="s">
         <v>21</v>
       </c>
@@ -4509,7 +4582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319">
+    <row r="319" spans="1:8" ht="13.2">
       <c r="A319" s="4" t="s">
         <v>21</v>
       </c>
@@ -4520,7 +4593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="320">
+    <row r="320" spans="1:8" ht="13.2">
       <c r="A320" s="4" t="s">
         <v>21</v>
       </c>
@@ -4528,7 +4601,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="321">
+    <row r="321" spans="1:8" ht="13.2">
       <c r="A321" s="4" t="s">
         <v>21</v>
       </c>
@@ -4539,7 +4612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322">
+    <row r="322" spans="1:8" ht="13.2">
       <c r="A322" s="4" t="s">
         <v>21</v>
       </c>
@@ -4547,7 +4620,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="323">
+    <row r="323" spans="1:8" ht="13.2">
       <c r="A323" s="4" t="s">
         <v>21</v>
       </c>
@@ -4558,7 +4631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324">
+    <row r="324" spans="1:8" ht="13.2">
       <c r="A324" s="4" t="s">
         <v>21</v>
       </c>
@@ -4569,7 +4642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325">
+    <row r="325" spans="1:8" ht="13.2">
       <c r="A325" s="4" t="s">
         <v>37</v>
       </c>
@@ -4577,7 +4650,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="326">
+    <row r="326" spans="1:8" ht="13.2">
       <c r="A326" s="4" t="s">
         <v>37</v>
       </c>
@@ -4591,7 +4664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327">
+    <row r="327" spans="1:8" ht="13.2">
       <c r="A327" s="4" t="s">
         <v>37</v>
       </c>
@@ -4602,7 +4675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="328">
+    <row r="328" spans="1:8" ht="13.2">
       <c r="A328" s="4" t="s">
         <v>37</v>
       </c>
@@ -4616,7 +4689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329">
+    <row r="329" spans="1:8" ht="13.2">
       <c r="A329" s="4" t="s">
         <v>37</v>
       </c>
@@ -4624,7 +4697,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="330">
+    <row r="330" spans="1:8" ht="13.2">
       <c r="A330" s="4" t="s">
         <v>37</v>
       </c>
@@ -4632,7 +4705,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="331">
+    <row r="331" spans="1:8" ht="13.2">
       <c r="A331" s="4" t="s">
         <v>37</v>
       </c>
@@ -4643,7 +4716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="332">
+    <row r="332" spans="1:8" ht="13.2">
       <c r="A332" s="4" t="s">
         <v>37</v>
       </c>
@@ -4657,7 +4730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333">
+    <row r="333" spans="1:8" ht="13.2">
       <c r="A333" s="4" t="s">
         <v>37</v>
       </c>
@@ -4665,7 +4738,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="334">
+    <row r="334" spans="1:8" ht="13.2">
       <c r="A334" s="4" t="s">
         <v>37</v>
       </c>
@@ -4676,12 +4749,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335">
+    <row r="335" spans="1:8" ht="13.2">
       <c r="F335" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="336">
+    <row r="336" spans="1:8" ht="13.8">
       <c r="B336" s="21" t="s">
         <v>322</v>
       </c>
@@ -4689,7 +4762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="337">
+    <row r="337" spans="1:8" ht="13.2">
       <c r="A337" s="4" t="s">
         <v>323</v>
       </c>
@@ -4697,7 +4770,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="338">
+    <row r="338" spans="1:8" ht="13.2">
       <c r="A338" s="4" t="s">
         <v>323</v>
       </c>
@@ -4705,7 +4778,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="339">
+    <row r="339" spans="1:8" ht="13.2">
       <c r="A339" s="4" t="s">
         <v>323</v>
       </c>
@@ -4719,7 +4792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="340">
+    <row r="340" spans="1:8" ht="13.2">
       <c r="A340" s="4" t="s">
         <v>323</v>
       </c>
@@ -4729,307 +4802,307 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B5"/>
-    <hyperlink r:id="rId2" ref="B6"/>
-    <hyperlink r:id="rId3" ref="B7"/>
-    <hyperlink r:id="rId4" ref="B8"/>
-    <hyperlink r:id="rId5" ref="B9"/>
-    <hyperlink r:id="rId6" ref="B10"/>
-    <hyperlink r:id="rId7" ref="B11"/>
-    <hyperlink r:id="rId8" ref="B12"/>
-    <hyperlink r:id="rId9" ref="B13"/>
-    <hyperlink r:id="rId10" ref="B14"/>
-    <hyperlink r:id="rId11" ref="B15"/>
-    <hyperlink r:id="rId12" ref="B16"/>
-    <hyperlink r:id="rId13" ref="B17"/>
-    <hyperlink r:id="rId14" ref="B18"/>
-    <hyperlink r:id="rId15" ref="B19"/>
-    <hyperlink r:id="rId16" ref="B20"/>
-    <hyperlink r:id="rId17" ref="B21"/>
-    <hyperlink r:id="rId18" ref="B22"/>
-    <hyperlink r:id="rId19" ref="B23"/>
-    <hyperlink r:id="rId20" ref="B24"/>
-    <hyperlink r:id="rId21" ref="B25"/>
-    <hyperlink r:id="rId22" ref="B26"/>
-    <hyperlink r:id="rId23" ref="B27"/>
-    <hyperlink r:id="rId24" ref="B28"/>
-    <hyperlink r:id="rId25" ref="B29"/>
-    <hyperlink r:id="rId26" ref="B30"/>
-    <hyperlink r:id="rId27" ref="B31"/>
-    <hyperlink r:id="rId28" ref="B32"/>
-    <hyperlink r:id="rId29" ref="B35"/>
-    <hyperlink r:id="rId30" ref="B36"/>
-    <hyperlink r:id="rId31" ref="B37"/>
-    <hyperlink r:id="rId32" ref="B38"/>
-    <hyperlink r:id="rId33" ref="B39"/>
-    <hyperlink r:id="rId34" ref="B40"/>
-    <hyperlink r:id="rId35" ref="B41"/>
-    <hyperlink r:id="rId36" ref="B42"/>
-    <hyperlink r:id="rId37" ref="B43"/>
-    <hyperlink r:id="rId38" ref="B44"/>
-    <hyperlink r:id="rId39" ref="B45"/>
-    <hyperlink r:id="rId40" ref="B46"/>
-    <hyperlink r:id="rId41" ref="B47"/>
-    <hyperlink r:id="rId42" ref="B48"/>
-    <hyperlink r:id="rId43" ref="B49"/>
-    <hyperlink r:id="rId44" ref="B50"/>
-    <hyperlink r:id="rId45" ref="B51"/>
-    <hyperlink r:id="rId46" ref="B52"/>
-    <hyperlink r:id="rId47" ref="B53"/>
-    <hyperlink r:id="rId48" ref="B54"/>
-    <hyperlink r:id="rId49" ref="B57"/>
-    <hyperlink r:id="rId50" ref="B58"/>
-    <hyperlink r:id="rId51" ref="B59"/>
-    <hyperlink r:id="rId52" ref="B60"/>
-    <hyperlink r:id="rId53" ref="B61"/>
-    <hyperlink r:id="rId54" ref="B64"/>
-    <hyperlink r:id="rId55" ref="B65"/>
-    <hyperlink r:id="rId56" ref="B66"/>
-    <hyperlink r:id="rId57" ref="B67"/>
-    <hyperlink r:id="rId58" ref="B68"/>
-    <hyperlink r:id="rId59" ref="B69"/>
-    <hyperlink r:id="rId60" ref="B70"/>
-    <hyperlink r:id="rId61" ref="B71"/>
-    <hyperlink r:id="rId62" ref="B72"/>
-    <hyperlink r:id="rId63" ref="B73"/>
-    <hyperlink r:id="rId64" ref="B74"/>
-    <hyperlink r:id="rId65" ref="B75"/>
-    <hyperlink r:id="rId66" ref="B78"/>
-    <hyperlink r:id="rId67" ref="B79"/>
-    <hyperlink r:id="rId68" ref="B80"/>
-    <hyperlink r:id="rId69" ref="B81"/>
-    <hyperlink r:id="rId70" ref="B82"/>
-    <hyperlink r:id="rId71" ref="B83"/>
-    <hyperlink r:id="rId72" ref="B84"/>
-    <hyperlink r:id="rId73" ref="B85"/>
-    <hyperlink r:id="rId74" ref="B86"/>
-    <hyperlink r:id="rId75" ref="B87"/>
-    <hyperlink r:id="rId76" ref="B88"/>
-    <hyperlink r:id="rId77" ref="B89"/>
-    <hyperlink r:id="rId78" ref="B90"/>
-    <hyperlink r:id="rId79" ref="B91"/>
-    <hyperlink r:id="rId80" ref="B92"/>
-    <hyperlink r:id="rId81" ref="B96"/>
-    <hyperlink r:id="rId82" ref="B97"/>
-    <hyperlink r:id="rId83" ref="B98"/>
-    <hyperlink r:id="rId84" ref="B99"/>
-    <hyperlink r:id="rId85" ref="B100"/>
-    <hyperlink r:id="rId86" ref="B101"/>
-    <hyperlink r:id="rId87" ref="B102"/>
-    <hyperlink r:id="rId88" ref="B103"/>
-    <hyperlink r:id="rId89" ref="B104"/>
-    <hyperlink r:id="rId90" ref="B105"/>
-    <hyperlink r:id="rId91" ref="B106"/>
-    <hyperlink r:id="rId92" ref="B107"/>
-    <hyperlink r:id="rId93" ref="B108"/>
-    <hyperlink r:id="rId94" ref="B109"/>
-    <hyperlink r:id="rId95" ref="B110"/>
-    <hyperlink r:id="rId96" ref="B111"/>
-    <hyperlink r:id="rId97" ref="B112"/>
-    <hyperlink r:id="rId98" ref="B113"/>
-    <hyperlink r:id="rId99" ref="B114"/>
-    <hyperlink r:id="rId100" ref="B115"/>
-    <hyperlink r:id="rId101" ref="B116"/>
-    <hyperlink r:id="rId102" ref="B117"/>
-    <hyperlink r:id="rId103" ref="B118"/>
-    <hyperlink r:id="rId104" ref="B119"/>
-    <hyperlink r:id="rId105" ref="B120"/>
-    <hyperlink r:id="rId106" ref="B121"/>
-    <hyperlink r:id="rId107" ref="B122"/>
-    <hyperlink r:id="rId108" ref="B123"/>
-    <hyperlink r:id="rId109" ref="B124"/>
-    <hyperlink r:id="rId110" ref="B125"/>
-    <hyperlink r:id="rId111" ref="B129"/>
-    <hyperlink r:id="rId112" ref="B130"/>
-    <hyperlink r:id="rId113" ref="B131"/>
-    <hyperlink r:id="rId114" ref="B132"/>
-    <hyperlink r:id="rId115" ref="B133"/>
-    <hyperlink r:id="rId116" ref="B134"/>
-    <hyperlink r:id="rId117" ref="B135"/>
-    <hyperlink r:id="rId118" ref="B136"/>
-    <hyperlink r:id="rId119" ref="B137"/>
-    <hyperlink r:id="rId120" ref="B138"/>
-    <hyperlink r:id="rId121" ref="B139"/>
-    <hyperlink r:id="rId122" ref="B140"/>
-    <hyperlink r:id="rId123" ref="B141"/>
-    <hyperlink r:id="rId124" ref="B142"/>
-    <hyperlink r:id="rId125" ref="B143"/>
-    <hyperlink r:id="rId126" ref="B144"/>
-    <hyperlink r:id="rId127" ref="B145"/>
-    <hyperlink r:id="rId128" ref="B146"/>
-    <hyperlink r:id="rId129" ref="B147"/>
-    <hyperlink r:id="rId130" ref="B148"/>
-    <hyperlink r:id="rId131" ref="B152"/>
-    <hyperlink r:id="rId132" ref="B153"/>
-    <hyperlink r:id="rId133" ref="B154"/>
-    <hyperlink r:id="rId134" ref="B155"/>
-    <hyperlink r:id="rId135" ref="B156"/>
-    <hyperlink r:id="rId136" ref="B157"/>
-    <hyperlink r:id="rId137" ref="B158"/>
-    <hyperlink r:id="rId138" ref="B159"/>
-    <hyperlink r:id="rId139" ref="B160"/>
-    <hyperlink r:id="rId140" ref="B161"/>
-    <hyperlink r:id="rId141" ref="B162"/>
-    <hyperlink r:id="rId142" ref="B163"/>
-    <hyperlink r:id="rId143" ref="B164"/>
-    <hyperlink r:id="rId144" ref="B165"/>
-    <hyperlink r:id="rId145" ref="B166"/>
-    <hyperlink r:id="rId146" ref="B167"/>
-    <hyperlink r:id="rId147" ref="B168"/>
-    <hyperlink r:id="rId148" ref="B169"/>
-    <hyperlink r:id="rId149" ref="B170"/>
-    <hyperlink r:id="rId150" ref="B171"/>
-    <hyperlink r:id="rId151" ref="B172"/>
-    <hyperlink r:id="rId152" ref="B173"/>
-    <hyperlink r:id="rId153" ref="B174"/>
-    <hyperlink r:id="rId154" ref="B175"/>
-    <hyperlink r:id="rId155" ref="B176"/>
-    <hyperlink r:id="rId156" ref="B177"/>
-    <hyperlink r:id="rId157" ref="B178"/>
-    <hyperlink r:id="rId158" ref="B179"/>
-    <hyperlink r:id="rId159" ref="B180"/>
-    <hyperlink r:id="rId160" ref="B181"/>
-    <hyperlink r:id="rId161" ref="B182"/>
-    <hyperlink r:id="rId162" ref="B183"/>
-    <hyperlink r:id="rId163" ref="B184"/>
-    <hyperlink r:id="rId164" ref="B185"/>
-    <hyperlink r:id="rId165" ref="B186"/>
-    <hyperlink r:id="rId166" ref="B187"/>
-    <hyperlink r:id="rId167" ref="B188"/>
-    <hyperlink r:id="rId168" ref="B189"/>
-    <hyperlink r:id="rId169" ref="B190"/>
-    <hyperlink r:id="rId170" ref="B191"/>
-    <hyperlink r:id="rId171" ref="B192"/>
-    <hyperlink r:id="rId172" ref="B193"/>
-    <hyperlink r:id="rId173" ref="B194"/>
-    <hyperlink r:id="rId174" ref="B195"/>
-    <hyperlink r:id="rId175" ref="B196"/>
-    <hyperlink r:id="rId176" ref="B197"/>
-    <hyperlink r:id="rId177" ref="B198"/>
-    <hyperlink r:id="rId178" ref="B199"/>
-    <hyperlink r:id="rId179" ref="B202"/>
-    <hyperlink r:id="rId180" ref="B203"/>
-    <hyperlink r:id="rId181" ref="B204"/>
-    <hyperlink r:id="rId182" ref="B205"/>
-    <hyperlink r:id="rId183" ref="B206"/>
-    <hyperlink r:id="rId184" ref="B207"/>
-    <hyperlink r:id="rId185" ref="B208"/>
-    <hyperlink r:id="rId186" ref="B209"/>
-    <hyperlink r:id="rId187" ref="B210"/>
-    <hyperlink r:id="rId188" ref="B211"/>
-    <hyperlink r:id="rId189" ref="B212"/>
-    <hyperlink r:id="rId190" ref="B213"/>
-    <hyperlink r:id="rId191" ref="B214"/>
-    <hyperlink r:id="rId192" ref="B215"/>
-    <hyperlink r:id="rId193" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." ref="B216"/>
-    <hyperlink r:id="rId194" ref="B217"/>
-    <hyperlink r:id="rId195" ref="B218"/>
-    <hyperlink r:id="rId196" ref="B219"/>
-    <hyperlink r:id="rId197" ref="B220"/>
-    <hyperlink r:id="rId198" ref="B221"/>
-    <hyperlink r:id="rId199" ref="B222"/>
-    <hyperlink r:id="rId200" ref="B223"/>
-    <hyperlink r:id="rId201" ref="B224"/>
-    <hyperlink r:id="rId202" ref="B225"/>
-    <hyperlink r:id="rId203" ref="B226"/>
-    <hyperlink r:id="rId204" ref="B227"/>
-    <hyperlink r:id="rId205" ref="B228"/>
-    <hyperlink r:id="rId206" ref="B229"/>
-    <hyperlink r:id="rId207" ref="B230"/>
-    <hyperlink r:id="rId208" ref="B231"/>
-    <hyperlink r:id="rId209" ref="B232"/>
-    <hyperlink r:id="rId210" ref="B233"/>
-    <hyperlink r:id="rId211" ref="B234"/>
-    <hyperlink r:id="rId212" ref="B235"/>
-    <hyperlink r:id="rId213" ref="B236"/>
-    <hyperlink r:id="rId214" ref="B237"/>
-    <hyperlink r:id="rId215" ref="B238"/>
-    <hyperlink r:id="rId216" ref="B241"/>
-    <hyperlink r:id="rId217" ref="B242"/>
-    <hyperlink r:id="rId218" ref="B243"/>
-    <hyperlink r:id="rId219" ref="B244"/>
-    <hyperlink r:id="rId220" ref="B245"/>
-    <hyperlink r:id="rId221" ref="B246"/>
-    <hyperlink r:id="rId222" ref="B250"/>
-    <hyperlink r:id="rId223" ref="B251"/>
-    <hyperlink r:id="rId224" ref="B252"/>
-    <hyperlink r:id="rId225" ref="B253"/>
-    <hyperlink r:id="rId226" ref="B254"/>
-    <hyperlink r:id="rId227" ref="B255"/>
-    <hyperlink r:id="rId228" ref="B256"/>
-    <hyperlink r:id="rId229" ref="B257"/>
-    <hyperlink r:id="rId230" ref="B258"/>
-    <hyperlink r:id="rId231" ref="B259"/>
-    <hyperlink r:id="rId232" ref="B260"/>
-    <hyperlink r:id="rId233" ref="B261"/>
-    <hyperlink r:id="rId234" ref="B262"/>
-    <hyperlink r:id="rId235" ref="B263"/>
-    <hyperlink r:id="rId236" ref="B266"/>
-    <hyperlink r:id="rId237" ref="B267"/>
-    <hyperlink r:id="rId238" ref="B268"/>
-    <hyperlink r:id="rId239" ref="B269"/>
-    <hyperlink r:id="rId240" ref="B270"/>
-    <hyperlink r:id="rId241" ref="B271"/>
-    <hyperlink r:id="rId242" ref="B272"/>
-    <hyperlink r:id="rId243" ref="B273"/>
-    <hyperlink r:id="rId244" ref="B274"/>
-    <hyperlink r:id="rId245" ref="B275"/>
-    <hyperlink r:id="rId246" ref="B276"/>
-    <hyperlink r:id="rId247" ref="B277"/>
-    <hyperlink r:id="rId248" ref="B278"/>
-    <hyperlink r:id="rId249" ref="B279"/>
-    <hyperlink r:id="rId250" ref="B280"/>
-    <hyperlink r:id="rId251" ref="B281"/>
-    <hyperlink r:id="rId252" ref="B282"/>
-    <hyperlink r:id="rId253" ref="B283"/>
-    <hyperlink r:id="rId254" ref="B284"/>
-    <hyperlink r:id="rId255" ref="B285"/>
-    <hyperlink r:id="rId256" ref="B286"/>
-    <hyperlink r:id="rId257" ref="B287"/>
-    <hyperlink r:id="rId258" ref="B288"/>
-    <hyperlink r:id="rId259" ref="B289"/>
-    <hyperlink r:id="rId260" ref="B290"/>
-    <hyperlink r:id="rId261" ref="B291"/>
-    <hyperlink r:id="rId262" ref="B292"/>
-    <hyperlink r:id="rId263" ref="B293"/>
-    <hyperlink r:id="rId264" ref="B294"/>
-    <hyperlink r:id="rId265" ref="B295"/>
-    <hyperlink r:id="rId266" ref="B298"/>
-    <hyperlink r:id="rId267" ref="B299"/>
-    <hyperlink r:id="rId268" ref="B300"/>
-    <hyperlink r:id="rId269" ref="B304"/>
-    <hyperlink r:id="rId270" ref="B305"/>
-    <hyperlink r:id="rId271" ref="B306"/>
-    <hyperlink r:id="rId272" ref="B307"/>
-    <hyperlink r:id="rId273" ref="B308"/>
-    <hyperlink r:id="rId274" ref="B309"/>
-    <hyperlink r:id="rId275" ref="B310"/>
-    <hyperlink r:id="rId276" ref="B311"/>
-    <hyperlink r:id="rId277" ref="B312"/>
-    <hyperlink r:id="rId278" ref="B313"/>
-    <hyperlink r:id="rId279" ref="B317"/>
-    <hyperlink r:id="rId280" ref="B318"/>
-    <hyperlink r:id="rId281" ref="B319"/>
-    <hyperlink r:id="rId282" ref="B320"/>
-    <hyperlink r:id="rId283" ref="B321"/>
-    <hyperlink r:id="rId284" ref="B322"/>
-    <hyperlink r:id="rId285" ref="B323"/>
-    <hyperlink r:id="rId286" ref="B324"/>
-    <hyperlink r:id="rId287" ref="B325"/>
-    <hyperlink r:id="rId288" ref="B326"/>
-    <hyperlink r:id="rId289" ref="B327"/>
-    <hyperlink r:id="rId290" ref="B328"/>
-    <hyperlink r:id="rId291" ref="B329"/>
-    <hyperlink r:id="rId292" ref="B330"/>
-    <hyperlink r:id="rId293" ref="B331"/>
-    <hyperlink r:id="rId294" ref="B332"/>
-    <hyperlink r:id="rId295" ref="B333"/>
-    <hyperlink r:id="rId296" ref="B334"/>
-    <hyperlink r:id="rId297" ref="B337"/>
-    <hyperlink r:id="rId298" ref="B338"/>
-    <hyperlink r:id="rId299" ref="B339"/>
-    <hyperlink r:id="rId300" ref="B340"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B35" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B36" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B38" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B39" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B41" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B42" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B43" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B44" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B45" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B46" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B47" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B48" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B49" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B50" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B51" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B52" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B53" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B54" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B57" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B58" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B59" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B60" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B61" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B64" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B65" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B66" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B67" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B68" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B69" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B70" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B71" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B72" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B73" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B74" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B75" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B78" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B79" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B80" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B81" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B82" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B83" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B84" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B85" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B86" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B87" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B88" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B89" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B90" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B91" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B92" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B96" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B97" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B98" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B99" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B100" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B101" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B102" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B103" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B104" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B105" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B106" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B107" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B108" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B109" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B110" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B111" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B112" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B113" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B114" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B115" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B116" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B117" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B118" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B119" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B120" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B121" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B122" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B123" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B124" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B125" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B129" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B130" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B131" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B132" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B133" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B134" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B135" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B136" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B137" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B138" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B139" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B140" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B141" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B142" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B143" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B144" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B145" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B146" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B147" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B148" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B152" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B153" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B154" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B155" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B156" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B157" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B158" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B159" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B160" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B161" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B162" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B163" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B164" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B165" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B166" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B167" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B168" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B169" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B170" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B171" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B172" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B173" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B174" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B175" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B176" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B177" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B178" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B179" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B180" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="B181" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B182" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B183" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B184" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B185" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B186" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B187" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B188" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B189" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B190" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B191" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B192" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B193" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B194" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B195" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B196" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="B197" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B198" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="B199" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B202" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="B203" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B204" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="B205" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B206" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="B207" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B208" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="B209" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B210" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="B211" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="B212" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="B213" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="B214" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="B215" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="B216" r:id="rId193" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="B217" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="B218" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="B219" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="B220" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="B221" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="B222" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="B223" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="B224" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="B225" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="B226" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="B227" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="B228" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="B229" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="B230" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="B231" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="B232" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="B233" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="B234" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="B235" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="B236" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="B237" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="B238" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="B241" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B242" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="B243" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B244" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="B245" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B246" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="B250" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="B251" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="B252" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="B253" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="B254" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="B255" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="B256" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="B257" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="B258" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="B259" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="B260" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="B261" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="B262" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="B263" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="B266" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="B267" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="B268" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="B269" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="B270" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="B271" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="B272" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="B273" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="B274" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="B275" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="B276" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="B277" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="B278" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="B279" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="B280" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="B281" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="B282" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="B283" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="B284" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="B285" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="B286" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="B287" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="B288" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="B289" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="B290" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="B291" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="B292" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="B293" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="B294" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="B295" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="B298" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="B299" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="B300" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="B304" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="B305" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="B306" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="B307" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="B308" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="B309" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="B310" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="B311" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="B312" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="B313" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="B317" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="B318" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="B319" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="B320" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="B321" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="B322" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="B323" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="B324" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="B325" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="B326" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="B327" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="B328" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="B329" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="B330" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="B331" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="B332" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="B333" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="B334" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="B337" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="B338" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="B339" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="B340" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
   </hyperlinks>
-  <drawing r:id="rId301"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DP 43 44 45 46 47 48
</commit_message>
<xml_diff>
--- a/DSA-280.xlsx
+++ b/DSA-280.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B2CC13-84EC-406C-9C1C-3DD20C2CA94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF384FB-2EA7-4EB8-9BCE-46D5A9DD5F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="328">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1430,8 +1430,8 @@
   </sheetPr>
   <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1643,6 +1643,9 @@
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="C16" t="s">
+        <v>327</v>
+      </c>
       <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
@@ -1685,6 +1688,9 @@
       <c r="B19" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="C19" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="13.2">
       <c r="A20" s="4" t="s">
@@ -1743,6 +1749,9 @@
       <c r="B24" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="C24" t="s">
+        <v>327</v>
+      </c>
       <c r="F24" s="4" t="s">
         <v>10</v>
       </c>
@@ -1753,6 +1762,9 @@
       </c>
       <c r="B25" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>327</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>10</v>

</xml_diff>